<commit_message>
new folder PROD visualizations, new graph Clubs_All, reworked visu
</commit_message>
<xml_diff>
--- a/zavodnici_exported.xlsx
+++ b/zavodnici_exported.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8AC2CA-B313-4319-AA20-ED79C14C2F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CB22DD-AEA2-4950-9568-3B497D622152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14616" yWindow="-16236" windowWidth="21384" windowHeight="15624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="-15240" windowWidth="19836" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2658,10 +2658,10 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="1">
@@ -2684,10 +2684,10 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C59" s="1">

</xml_diff>